<commit_message>
fetch data file from windows before running to ensure up-to-date data
</commit_message>
<xml_diff>
--- a/my-first-app/data.xlsx
+++ b/my-first-app/data.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andbra\AppData\Local\Packages\CanonicalGroupLimited.Ubuntu22.04LTS_79rhkp1fndgsc\LocalState\rootfs\home\andbra\dev\private\streamlit-apps\my-first-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A65244E-7907-4A7E-8FED-9A59CBCF2030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{4A65244E-7907-4A7E-8FED-9A59CBCF2030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7892BAB-AC2F-044E-A3E1-7DE436A2D629}"/>
   <bookViews>
     <workbookView xWindow="4290" yWindow="4290" windowWidth="7380" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -384,17 +397,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="18.29296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.14453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -404,7 +417,7 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>44927</v>
       </c>
@@ -415,7 +428,7 @@
         <v>119.6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>44928</v>
       </c>
@@ -426,7 +439,7 @@
         <v>119.6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>44929</v>
       </c>
@@ -437,7 +450,7 @@
         <v>119.6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>44930</v>
       </c>
@@ -448,7 +461,7 @@
         <v>119.6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>44931</v>
       </c>
@@ -459,7 +472,7 @@
         <v>119.6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>44932</v>
       </c>
@@ -470,7 +483,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>44933</v>
       </c>
@@ -481,7 +494,7 @@
         <v>119.5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>44934</v>
       </c>
@@ -492,7 +505,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>44935</v>
       </c>
@@ -503,7 +516,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>44936</v>
       </c>
@@ -514,7 +527,7 @@
         <v>119.3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>44937</v>
       </c>
@@ -525,7 +538,7 @@
         <v>119.6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>44938</v>
       </c>
@@ -536,7 +549,7 @@
         <v>119.6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>44939</v>
       </c>
@@ -547,7 +560,7 @@
         <v>119.6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>44940</v>
       </c>
@@ -558,7 +571,7 @@
         <v>119.6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>44941</v>
       </c>
@@ -569,7 +582,7 @@
         <v>119.2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>44942</v>
       </c>
@@ -580,7 +593,7 @@
         <v>120.1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>44943</v>
       </c>
@@ -591,7 +604,7 @@
         <v>121.1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>44944</v>
       </c>
@@ -602,7 +615,7 @@
         <v>120.7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>44945</v>
       </c>
@@ -613,7 +626,7 @@
         <v>120.9</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>44946</v>
       </c>
@@ -624,7 +637,7 @@
         <v>121.1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>44947</v>
       </c>
@@ -635,7 +648,7 @@
         <v>120.7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>44948</v>
       </c>
@@ -646,7 +659,7 @@
         <v>120.3</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>44949</v>
       </c>
@@ -657,7 +670,7 @@
         <v>119.9</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>44950</v>
       </c>
@@ -668,7 +681,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>44951</v>
       </c>
@@ -679,7 +692,7 @@
         <v>120.2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>44952</v>
       </c>
@@ -690,7 +703,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>44953</v>
       </c>
@@ -701,7 +714,7 @@
         <v>120.55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>44954</v>
       </c>
@@ -712,7 +725,7 @@
         <v>120.1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>44955</v>
       </c>
@@ -723,7 +736,7 @@
         <v>119.5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>44956</v>
       </c>
@@ -734,7 +747,7 @@
         <v>118.5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>44957</v>
       </c>
@@ -745,7 +758,7 @@
         <v>118.9</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>44958</v>
       </c>
@@ -756,7 +769,7 @@
         <v>118.9</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>44959</v>
       </c>
@@ -767,7 +780,7 @@
         <v>118.5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>44960</v>
       </c>
@@ -778,7 +791,7 @@
         <v>119.4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>44961</v>
       </c>
@@ -789,7 +802,7 @@
         <v>118.9</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>44962</v>
       </c>
@@ -800,7 +813,7 @@
         <v>118.9</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>44963</v>
       </c>
@@ -811,7 +824,7 @@
         <v>117.8</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>44964</v>
       </c>
@@ -822,7 +835,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>44965</v>
       </c>
@@ -833,7 +846,7 @@
         <v>117.2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>44966</v>
       </c>
@@ -844,7 +857,7 @@
         <v>118.3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>44967</v>
       </c>
@@ -855,7 +868,7 @@
         <v>119.8</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>44968</v>
       </c>
@@ -866,7 +879,7 @@
         <v>117.5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>44969</v>
       </c>
@@ -877,7 +890,7 @@
         <v>118.6</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>44970</v>
       </c>
@@ -888,7 +901,7 @@
         <v>118.7</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>44971</v>
       </c>
@@ -899,7 +912,7 @@
         <v>118.3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>44972</v>
       </c>
@@ -910,7 +923,7 @@
         <v>118.1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>44973</v>
       </c>
@@ -921,7 +934,7 @@
         <v>117.9</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>44974</v>
       </c>
@@ -932,7 +945,7 @@
         <v>118.6</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>44975</v>
       </c>
@@ -943,7 +956,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>44976</v>
       </c>
@@ -954,7 +967,7 @@
         <v>118.4</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3">
         <v>44977</v>
       </c>
@@ -965,7 +978,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3">
         <v>44978</v>
       </c>
@@ -976,7 +989,7 @@
         <v>119.2</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3">
         <v>44979</v>
       </c>
@@ -987,7 +1000,7 @@
         <v>119.5</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3">
         <v>44980</v>
       </c>
@@ -998,7 +1011,7 @@
         <v>119.3</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3">
         <v>44981</v>
       </c>
@@ -1009,7 +1022,7 @@
         <v>119.2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3">
         <v>44982</v>
       </c>
@@ -1020,7 +1033,7 @@
         <v>118.2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3">
         <v>44983</v>
       </c>
@@ -1031,7 +1044,7 @@
         <v>117.9</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3">
         <v>44984</v>
       </c>
@@ -1042,7 +1055,7 @@
         <v>118.5</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="3">
         <v>44985</v>
       </c>
@@ -1053,7 +1066,7 @@
         <v>118.4</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="3">
         <v>44986</v>
       </c>
@@ -1064,7 +1077,7 @@
         <v>118.4</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="3">
         <v>44987</v>
       </c>
@@ -1075,7 +1088,7 @@
         <v>118.4</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="3">
         <v>44988</v>
       </c>
@@ -1086,7 +1099,7 @@
         <v>118.4</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="3">
         <v>44989</v>
       </c>
@@ -1097,7 +1110,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="3">
         <v>44990</v>
       </c>
@@ -1108,531 +1121,536 @@
         <v>117.2</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="3">
         <v>44991</v>
       </c>
       <c r="B66" s="4">
         <v>115.8</v>
       </c>
-      <c r="C66" s="4"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="4">
+        <v>116.9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="3">
         <v>44992</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="3">
         <v>44993</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="3">
         <v>44994</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="3">
         <v>44995</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="3">
         <v>44996</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>44997</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="3">
         <v>44998</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="3">
         <v>44999</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="3">
         <v>45000</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="3">
         <v>45001</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="3">
         <v>45002</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="3">
         <v>45003</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="3">
         <v>45004</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="3">
         <v>45005</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="3">
         <v>45006</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="3">
         <v>45007</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="3">
         <v>45008</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="3">
         <v>45009</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="3">
         <v>45010</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="3">
         <v>45011</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="3">
         <v>45012</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="3">
         <v>45013</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="3">
         <v>45014</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="3">
         <v>45015</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="3">
         <v>45016</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="3">
         <v>45017</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="3">
         <v>45018</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="3">
         <v>45019</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="3">
         <v>45020</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="3">
         <v>45021</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="3">
         <v>45022</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="3">
         <v>45023</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="3">
         <v>45024</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="3">
         <v>45025</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="3">
         <v>45026</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="3">
         <v>45027</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="3">
         <v>45028</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" s="3">
         <v>45029</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="3">
         <v>45030</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="3">
         <v>45031</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="3">
         <v>45032</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="3">
         <v>45033</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="3">
         <v>45034</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="3">
         <v>45035</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="3">
         <v>45036</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" s="3">
         <v>45037</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="3">
         <v>45038</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="3">
         <v>45039</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="3">
         <v>45040</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="3">
         <v>45041</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="3">
         <v>45042</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="3">
         <v>45043</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="3">
         <v>45044</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="3">
         <v>45045</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="3">
         <v>45046</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="3">
         <v>45047</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="3">
         <v>45048</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="3">
         <v>45049</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="3">
         <v>45050</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="3">
         <v>45051</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="3">
         <v>45052</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="3">
         <v>45053</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="3">
         <v>45054</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="3">
         <v>45055</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="3">
         <v>45056</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="3">
         <v>45057</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="3">
         <v>45058</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="3">
         <v>45059</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="3">
         <v>45060</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" s="3">
         <v>45061</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="3">
         <v>45062</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="3">
         <v>45063</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="3">
         <v>45064</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="3">
         <v>45065</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" s="3">
         <v>45066</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" s="3">
         <v>45067</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" s="3">
         <v>45068</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" s="3">
         <v>45069</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="3">
         <v>45070</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="3">
         <v>45071</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="3">
         <v>45072</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="3">
         <v>45073</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="3">
         <v>45074</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="3">
         <v>45075</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="3">
         <v>45076</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" s="3">
         <v>45077</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" s="3">
         <v>45078</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" s="3">
         <v>45079</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" s="3">
         <v>45080</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" s="3">
         <v>45081</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" s="3">
         <v>45082</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" s="3">
         <v>45083</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" s="3">
         <v>45084</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="3">
         <v>45085</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" s="3">
         <v>45086</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" s="3">
         <v>45087</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" s="3">
         <v>45088</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" s="3">
         <v>45089</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" s="3">
         <v>45090</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" s="3">
         <v>45091</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" s="3">
         <v>45092</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" s="3">
         <v>45093</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" s="3">
         <v>45094</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" s="3">
         <v>45095</v>
       </c>

</xml_diff>

<commit_message>
update data and fig
</commit_message>
<xml_diff>
--- a/my-first-app/data.xlsx
+++ b/my-first-app/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andbra\AppData\Local\Packages\CanonicalGroupLimited.Ubuntu22.04LTS_79rhkp1fndgsc\LocalState\rootfs\home\andbra\dev\private\streamlit-apps\my-first-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{4A65244E-7907-4A7E-8FED-9A59CBCF2030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FE18D68-9160-B541-998E-F3C731422C58}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{4A65244E-7907-4A7E-8FED-9A59CBCF2030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A072B0E-CC98-ED4A-B4EC-EDC6E85E34B5}"/>
   <bookViews>
     <workbookView xWindow="4290" yWindow="4290" windowWidth="7380" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1180,10 +1180,22 @@
       <c r="A71" s="3">
         <v>44996</v>
       </c>
+      <c r="B71" s="1">
+        <v>116.1</v>
+      </c>
+      <c r="C71" s="1">
+        <v>116.7</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="3">
         <v>44997</v>
+      </c>
+      <c r="B72" s="1">
+        <v>115.7</v>
+      </c>
+      <c r="C72" s="1">
+        <v>116.9</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>